<commit_message>
modified the rest of on_click events from containers into buttons
</commit_message>
<xml_diff>
--- a/WalkingApp/walking_data.xlsx
+++ b/WalkingApp/walking_data.xlsx
@@ -63,15 +63,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="#,##0_ "/>
-    <numFmt numFmtId="177" formatCode="h:mm;@"/>
-    <numFmt numFmtId="178" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="176" formatCode="h:mm;@"/>
+    <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="179" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="180" formatCode="#,##0_ "/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="hh:mm:ss;@"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -90,14 +90,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -105,38 +150,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -152,83 +176,59 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,25 +255,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,157 +417,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,8 +531,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -554,24 +578,35 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,188 +625,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="15">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="15">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -779,49 +779,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -833,10 +833,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1173,7 +1173,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
solved problem with time entry and it's ValueError time data does not match required format
</commit_message>
<xml_diff>
--- a/WalkingApp/walking_data.xlsx
+++ b/WalkingApp/walking_data.xlsx
@@ -63,15 +63,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
     <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="178" formatCode="0.00_ "/>
-    <numFmt numFmtId="179" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="h:mm;@"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="#,##0_ "/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -87,6 +87,81 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -99,13 +174,14 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -113,6 +189,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -123,112 +207,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,13 +255,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +297,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +321,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,145 +393,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,15 +537,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -562,16 +553,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,23 +596,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -630,148 +630,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="15">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -779,7 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,16 +788,16 @@
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -806,19 +806,19 @@
     <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -833,10 +833,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1173,7 +1173,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H26" sqref="A21:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
Added some modifications - e.g. list comprehensions - to fill_table() and data_for_table() functions
</commit_message>
<xml_diff>
--- a/WalkingApp/walking_data.xlsx
+++ b/WalkingApp/walking_data.xlsx
@@ -60,14 +60,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
-    <numFmt numFmtId="177" formatCode="#,##0_ "/>
-    <numFmt numFmtId="178" formatCode="hh:mm:ss;@"/>
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
+    <numFmt numFmtId="177" formatCode="hh:mm:ss;@"/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="179" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="180" formatCode="h:mm;@"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -95,8 +95,99 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,121 +202,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,13 +240,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,19 +300,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,145 +420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,20 +462,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -491,6 +488,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,23 +545,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,121 +564,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="7">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
@@ -687,19 +687,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
@@ -713,22 +713,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -736,23 +733,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,7 +760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1097,7 +1097,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G22" sqref="A19:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>

</xml_diff>